<commit_message>
Adding excel example to deck
</commit_message>
<xml_diff>
--- a/Silas.Deck/SampleForecast.xlsx
+++ b/Silas.Deck/SampleForecast.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38355" yWindow="-435" windowWidth="38265" windowHeight="23940" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="-38355" yWindow="-435" windowWidth="38265" windowHeight="23940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="InitData" localSheetId="0">Sheet1!$A$2:$B$100</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$F$1</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$F$1</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -31,13 +32,14 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!#REF!</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$D$103</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">0.8</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">0.1</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">0.9</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">0.9</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -47,7 +49,7 @@
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -566,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -583,7 +585,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="5">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -638,11 +640,11 @@
       </c>
       <c r="C5" s="3">
         <f>$F$1*$B4 + (1-$F$1)*$C4</f>
-        <v>3143.4</v>
+        <v>3516</v>
       </c>
       <c r="D5" s="4">
-        <f>C5-B5</f>
-        <v>-2339.6</v>
+        <f>ABS(C5-B5)</f>
+        <v>1967</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1594,6 +1596,10 @@
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="4"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C101" s="3"/>
+      <c r="D101" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>